<commit_message>
lambda let examples, and encoding when replacing in powershell
</commit_message>
<xml_diff>
--- a/excel/LAMBDA_and_LET_in_Excel_examples.xlsx
+++ b/excel/LAMBDA_and_LET_in_Excel_examples.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonb\Dropbox\secretGeek\gh\util\TIL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F49C7C-405F-479D-B643-D0B9127C7690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF48569-E662-4CA3-8936-9EDD5009FBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="23226" windowHeight="13866" xr2:uid="{16B4DA44-29F7-4745-8BDB-2360DC2E66E9}"/>
+    <workbookView minimized="1" xWindow="2513" yWindow="2513" windowWidth="17280" windowHeight="9980" xr2:uid="{16B4DA44-29F7-4745-8BDB-2360DC2E66E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="BlockVolume">_xlfn.LAMBDA(_xlpm.a,_xlpm.b,_xlpm.c,_xlpm.a*_xlpm.b*_xlpm.c)</definedName>
+    <definedName name="BlockVolume2">_xlfn.LAMBDA(_xlpm.height,_xlpm.width,_xlpm.length,   _xlfn.LET(  _xlpm.volume, _xlpm.height * _xlpm.width * _xlpm.length,  _xlpm.volume   ) )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>BLOCKS</t>
   </si>
@@ -76,6 +77,18 @@
   </si>
   <si>
     <t>Volume</t>
+  </si>
+  <si>
+    <t>Volume2</t>
+  </si>
+  <si>
+    <t>Volume3</t>
+  </si>
+  <si>
+    <t>Volume 4</t>
+  </si>
+  <si>
+    <t>Volume 5</t>
   </si>
 </sst>
 </file>
@@ -111,13 +124,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -135,14 +161,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7289075D-CDA7-490F-9D96-B71C83CBC7D4}" name="Table1" displayName="Table1" ref="C3:F14" totalsRowShown="0">
-  <autoFilter ref="C3:F14" xr:uid="{7289075D-CDA7-490F-9D96-B71C83CBC7D4}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7289075D-CDA7-490F-9D96-B71C83CBC7D4}" name="Table1" displayName="Table1" ref="C3:J14" totalsRowShown="0">
+  <autoFilter ref="C3:J14" xr:uid="{7289075D-CDA7-490F-9D96-B71C83CBC7D4}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{07E75751-0CF3-4D50-9CDD-DCAB7D07B0AC}" name="Width"/>
     <tableColumn id="2" xr3:uid="{0FB79B1F-A733-435A-8314-113BF8A9963B}" name="Height"/>
     <tableColumn id="3" xr3:uid="{3C929B74-8F33-47EB-98B8-387F08919089}" name="Depth"/>
-    <tableColumn id="4" xr3:uid="{158BEC6F-1E60-4BAE-9AAB-9E26E9E4F43C}" name="Volume" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{158BEC6F-1E60-4BAE-9AAB-9E26E9E4F43C}" name="Volume" dataDxfId="4">
       <calculatedColumnFormula array="1">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{29BA4957-1CDE-4143-A033-853C2F0AF38E}" name="Volume2" dataDxfId="3">
+      <calculatedColumnFormula array="1">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C4,D4,E4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C9317686-B841-450A-94B1-40069E19897C}" name="Volume3" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.LET(_xlpm.x,C4,_xlpm.y,D4,_xlpm.z,E4,_xlpm.volume, _xlpm.x*_xlpm.y*_xlpm.z,_xlpm.volume)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{39FDAD21-F007-4B11-AE90-FC12735AE00C}" name="Volume 4" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.LET(_xlpm.x,C4,_xlpm.y,D4,_xlpm.z,E4,_xlpm.x*_xlpm.y*_xlpm.z)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{1C44BEFC-8A71-4696-A689-2BD66B48684C}" name="Volume 5" dataDxfId="0">
+      <calculatedColumnFormula array="1">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -466,20 +504,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30C929E-AB45-4751-B0D9-EDC6E21ACADF}">
-  <dimension ref="C1:F14"/>
+  <dimension ref="C1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="7.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.8203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.1171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.46875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -492,8 +538,20 @@
       <c r="F3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C4">
         <v>1</v>
       </c>
@@ -507,8 +565,24 @@
         <f t="array" ref="F4">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="G4" cm="1">
+        <f t="array" ref="G4">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C4,D4,E4)</f>
+        <v>28</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H14" si="0">_xlfn.LET(_xlpm.x,C4,_xlpm.y,D4,_xlpm.z,E4,_xlpm.volume, _xlpm.x*_xlpm.y*_xlpm.z,_xlpm.volume)</f>
+        <v>28</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I14" si="1">_xlfn.LET(_xlpm.x,C4,_xlpm.y,D4,_xlpm.z,E4,_xlpm.x*_xlpm.y*_xlpm.z)</f>
+        <v>28</v>
+      </c>
+      <c r="J4" cm="1">
+        <f t="array" ref="J4">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C5">
         <v>2</v>
       </c>
@@ -522,8 +596,24 @@
         <f t="array" ref="F5">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="G5" cm="1">
+        <f t="array" ref="G5">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C5,D5,E5)</f>
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="J5" s="1" cm="1">
+        <f t="array" ref="J5">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C6">
         <v>3</v>
       </c>
@@ -531,14 +621,30 @@
         <v>6</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F6" cm="1">
         <f t="array" ref="F6">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.5">
+        <v>216</v>
+      </c>
+      <c r="G6" cm="1">
+        <f t="array" ref="G6">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C6,D6,E6)</f>
+        <v>216</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>216</v>
+      </c>
+      <c r="J6" s="1" cm="1">
+        <f t="array" ref="J6">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C7">
         <v>4</v>
       </c>
@@ -552,8 +658,24 @@
         <f t="array" ref="F7">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
         <v>280</v>
       </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="G7" cm="1">
+        <f t="array" ref="G7">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C7,D7,E7)</f>
+        <v>280</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+      <c r="J7" s="1" cm="1">
+        <f t="array" ref="J7">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C8">
         <v>5</v>
       </c>
@@ -567,8 +689,24 @@
         <f t="array" ref="F8">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
         <v>440</v>
       </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="G8" cm="1">
+        <f t="array" ref="G8">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C8,D8,E8)</f>
+        <v>440</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>440</v>
+      </c>
+      <c r="J8" s="1" cm="1">
+        <f t="array" ref="J8">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C9">
         <v>6</v>
       </c>
@@ -576,14 +714,30 @@
         <v>9</v>
       </c>
       <c r="E9">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F9" cm="1">
         <f t="array" ref="F9">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
-        <v>648</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.5">
+        <v>432</v>
+      </c>
+      <c r="G9" cm="1">
+        <f t="array" ref="G9">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C9,D9,E9)</f>
+        <v>432</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>432</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>432</v>
+      </c>
+      <c r="J9" s="1" cm="1">
+        <f t="array" ref="J9">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C10">
         <v>7</v>
       </c>
@@ -597,8 +751,24 @@
         <f t="array" ref="F10">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
         <v>910</v>
       </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="G10" cm="1">
+        <f t="array" ref="G10">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C10,D10,E10)</f>
+        <v>910</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>910</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>910</v>
+      </c>
+      <c r="J10" s="1" cm="1">
+        <f t="array" ref="J10">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>910</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C11">
         <v>8</v>
       </c>
@@ -606,14 +776,30 @@
         <v>11</v>
       </c>
       <c r="E11">
-        <v>14</v>
+        <v>721</v>
       </c>
       <c r="F11" cm="1">
         <f t="array" ref="F11">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.5">
+        <v>63448</v>
+      </c>
+      <c r="G11" cm="1">
+        <f t="array" ref="G11">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C11,D11,E11)</f>
+        <v>63448</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>63448</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>63448</v>
+      </c>
+      <c r="J11" s="1" cm="1">
+        <f t="array" ref="J11">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>63448</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C12">
         <v>9</v>
       </c>
@@ -627,8 +813,24 @@
         <f t="array" ref="F12">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
         <v>1620</v>
       </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="G12" cm="1">
+        <f t="array" ref="G12">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C12,D12,E12)</f>
+        <v>1620</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1620</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>1620</v>
+      </c>
+      <c r="J12" s="1" cm="1">
+        <f t="array" ref="J12">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C13">
         <v>10</v>
       </c>
@@ -642,8 +844,24 @@
         <f t="array" ref="F13">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
         <v>2080</v>
       </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="G13" cm="1">
+        <f t="array" ref="G13">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C13,D13,E13)</f>
+        <v>2080</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>2080</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>2080</v>
+      </c>
+      <c r="J13" s="1" cm="1">
+        <f t="array" ref="J13">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C14">
         <v>11</v>
       </c>
@@ -655,6 +873,22 @@
       </c>
       <c r="F14" cm="1">
         <f t="array" ref="F14">BlockVolume(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
+        <v>2618</v>
+      </c>
+      <c r="G14" cm="1">
+        <f t="array" ref="G14">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.x*_xlpm.y*_xlpm.z)(C14,D14,E14)</f>
+        <v>2618</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>2618</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>2618</v>
+      </c>
+      <c r="J14" s="1" cm="1">
+        <f t="array" ref="J14">BlockVolume2(Table1[[#This Row],[Width]],Table1[[#This Row],[Height]],Table1[[#This Row],[Depth]])</f>
         <v>2618</v>
       </c>
     </row>

</xml_diff>